<commit_message>
another test data fix
</commit_message>
<xml_diff>
--- a/test_uploads/new_test_data_multipage.xlsx
+++ b/test_uploads/new_test_data_multipage.xlsx
@@ -47,9 +47,6 @@
     <t>original country fishing</t>
   </si>
   <si>
-    <t>original sector</t>
-  </si>
-  <si>
     <t>EEZ sub area</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>province state</t>
+  </si>
+  <si>
+    <t>original sector</t>
   </si>
   <si>
     <t>original taxon name</t>
@@ -1691,12 +1691,12 @@
         <v>29</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" t="s" s="6">
-        <v>30</v>
-      </c>
+      <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="O2" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
@@ -1743,12 +1743,12 @@
         <v>29</v>
       </c>
       <c r="K3" s="10"/>
-      <c r="L3" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="O3" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
@@ -1795,12 +1795,12 @@
         <v>29</v>
       </c>
       <c r="K4" s="10"/>
-      <c r="L4" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="O4" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -1847,12 +1847,12 @@
         <v>29</v>
       </c>
       <c r="K5" s="10"/>
-      <c r="L5" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="O5" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
@@ -1899,12 +1899,12 @@
         <v>29</v>
       </c>
       <c r="K6" s="10"/>
-      <c r="L6" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="O6" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
@@ -1951,12 +1951,12 @@
         <v>29</v>
       </c>
       <c r="K7" s="10"/>
-      <c r="L7" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="O7" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
@@ -2003,12 +2003,12 @@
         <v>29</v>
       </c>
       <c r="K8" s="10"/>
-      <c r="L8" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="O8" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
@@ -2055,12 +2055,12 @@
         <v>29</v>
       </c>
       <c r="K9" s="10"/>
-      <c r="L9" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="O9" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -2107,12 +2107,12 @@
         <v>29</v>
       </c>
       <c r="K10" s="10"/>
-      <c r="L10" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="O10" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -2159,12 +2159,12 @@
         <v>29</v>
       </c>
       <c r="K11" s="10"/>
-      <c r="L11" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="O11" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -2211,12 +2211,12 @@
         <v>29</v>
       </c>
       <c r="K12" s="10"/>
-      <c r="L12" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="O12" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
@@ -2263,12 +2263,12 @@
         <v>29</v>
       </c>
       <c r="K13" s="10"/>
-      <c r="L13" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="O13" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
@@ -2315,12 +2315,12 @@
         <v>29</v>
       </c>
       <c r="K14" s="10"/>
-      <c r="L14" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="O14" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
@@ -2367,12 +2367,12 @@
         <v>29</v>
       </c>
       <c r="K15" s="10"/>
-      <c r="L15" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="O15" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -2419,12 +2419,12 @@
         <v>29</v>
       </c>
       <c r="K16" s="10"/>
-      <c r="L16" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
+      <c r="O16" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
@@ -2471,12 +2471,12 @@
         <v>29</v>
       </c>
       <c r="K17" s="10"/>
-      <c r="L17" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="O17" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
@@ -2523,12 +2523,12 @@
         <v>29</v>
       </c>
       <c r="K18" s="10"/>
-      <c r="L18" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="O18" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
@@ -2575,12 +2575,12 @@
         <v>29</v>
       </c>
       <c r="K19" s="10"/>
-      <c r="L19" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="O19" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
@@ -2627,12 +2627,12 @@
         <v>29</v>
       </c>
       <c r="K20" s="10"/>
-      <c r="L20" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
+      <c r="O20" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
@@ -2679,12 +2679,12 @@
         <v>29</v>
       </c>
       <c r="K21" s="10"/>
-      <c r="L21" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="O21" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
@@ -2731,12 +2731,12 @@
         <v>29</v>
       </c>
       <c r="K22" s="10"/>
-      <c r="L22" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="O22" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
@@ -2783,12 +2783,12 @@
         <v>29</v>
       </c>
       <c r="K23" s="10"/>
-      <c r="L23" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="O23" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
@@ -2835,12 +2835,12 @@
         <v>29</v>
       </c>
       <c r="K24" s="10"/>
-      <c r="L24" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="O24" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
@@ -2887,12 +2887,12 @@
         <v>29</v>
       </c>
       <c r="K25" s="10"/>
-      <c r="L25" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="O25" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
@@ -2939,12 +2939,12 @@
         <v>29</v>
       </c>
       <c r="K26" s="10"/>
-      <c r="L26" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
+      <c r="O26" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
@@ -2991,12 +2991,12 @@
         <v>29</v>
       </c>
       <c r="K27" s="10"/>
-      <c r="L27" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
+      <c r="O27" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -3043,12 +3043,12 @@
         <v>29</v>
       </c>
       <c r="K28" s="10"/>
-      <c r="L28" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
+      <c r="O28" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
@@ -3095,12 +3095,12 @@
         <v>29</v>
       </c>
       <c r="K29" s="10"/>
-      <c r="L29" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
+      <c r="O29" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
@@ -3147,12 +3147,12 @@
         <v>29</v>
       </c>
       <c r="K30" s="10"/>
-      <c r="L30" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+      <c r="O30" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
@@ -3199,12 +3199,12 @@
         <v>29</v>
       </c>
       <c r="K31" s="10"/>
-      <c r="L31" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
+      <c r="O31" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
@@ -3251,12 +3251,12 @@
         <v>29</v>
       </c>
       <c r="K32" s="10"/>
-      <c r="L32" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
+      <c r="O32" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
@@ -3303,12 +3303,12 @@
         <v>29</v>
       </c>
       <c r="K33" s="10"/>
-      <c r="L33" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
+      <c r="O33" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
@@ -3355,12 +3355,12 @@
         <v>29</v>
       </c>
       <c r="K34" s="10"/>
-      <c r="L34" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
+      <c r="O34" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
@@ -3407,12 +3407,12 @@
         <v>29</v>
       </c>
       <c r="K35" s="10"/>
-      <c r="L35" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
+      <c r="O35" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
@@ -3459,12 +3459,12 @@
         <v>29</v>
       </c>
       <c r="K36" s="10"/>
-      <c r="L36" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
+      <c r="O36" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
@@ -3511,12 +3511,12 @@
         <v>29</v>
       </c>
       <c r="K37" s="10"/>
-      <c r="L37" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
+      <c r="O37" t="s" s="9">
+        <v>30</v>
+      </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>

</xml_diff>